<commit_message>
am implementat email ul
</commit_message>
<xml_diff>
--- a/Data/rpa_project.xlsx
+++ b/Data/rpa_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\OneDrive\Desktop\RPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ANUL III\RPA\rpa_project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33E3C835-8069-4569-B746-BD8009C5FBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0B3F06-7C0A-4B8F-9DB7-2891F55770C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0FD55BF-3B9A-4A67-AAC8-5CF92D9143BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Galatan Tudor</t>
   </si>
@@ -53,7 +53,13 @@
     <t>marinescudragos2014@gmail.com</t>
   </si>
   <si>
-    <t>parnau.patrick@yahoo.com</t>
+    <t>parnaumark17@gmail.com</t>
+  </si>
+  <si>
+    <t>Nume</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -438,26 +444,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04D1A62-1D83-4DD7-AC5D-AD2ADC705185}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.796875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -465,17 +471,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{4D6B0D86-1179-4BA7-8CD4-3C89AFBFB669}"/>
+    <hyperlink ref="B1" r:id="rId1" display="galatan.tudor1@gmail.com" xr:uid="{4D6B0D86-1179-4BA7-8CD4-3C89AFBFB669}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{97173D32-ED3C-4DFA-9074-DD2FC90AC4BD}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{F92574DC-E834-419C-AEFF-E34BD5860C5A}"/>
   </hyperlinks>

</xml_diff>